<commit_message>
Added RC2014 720k format
</commit_message>
<xml_diff>
--- a/DiskUtility/Notes/Skew Table.xlsx
+++ b/DiskUtility/Notes/Skew Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\Github\DiskImageUtility\DiskUtility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\Github\DiskImageUtility\DiskUtility\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B232DA4E-914C-409B-9DA7-11614A7D6398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFDF1A5-D5E9-4925-8DD9-CC3D4C472737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31995" yWindow="1725" windowWidth="25470" windowHeight="11835" activeTab="3" xr2:uid="{DD7A5C08-DCA6-4B6E-BD23-734986915BC7}"/>
+    <workbookView xWindow="29955" yWindow="3420" windowWidth="21600" windowHeight="11385" activeTab="8" xr2:uid="{DD7A5C08-DCA6-4B6E-BD23-734986915BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Skew" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Ext" sheetId="3" r:id="rId6"/>
     <sheet name="FAT" sheetId="5" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
+    <sheet name="RC2014" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="267">
   <si>
     <t>Skew</t>
   </si>
@@ -794,6 +795,54 @@
   </si>
   <si>
     <t>LLL Format</t>
+  </si>
+  <si>
+    <t>RC2014</t>
+  </si>
+  <si>
+    <t>H-37 800k</t>
+  </si>
+  <si>
+    <t>DIR Start</t>
+  </si>
+  <si>
+    <t>Sec Size</t>
+  </si>
+  <si>
+    <t>Hd</t>
+  </si>
+  <si>
+    <t>First File ALB</t>
+  </si>
+  <si>
+    <t>Reserved Trks</t>
+  </si>
+  <si>
+    <t>1st ALB</t>
+  </si>
+  <si>
+    <t>Track Cnt</t>
+  </si>
+  <si>
+    <t>Track Size</t>
+  </si>
+  <si>
+    <t>Dir ALB Start</t>
+  </si>
+  <si>
+    <t>Dir ALB Last</t>
+  </si>
+  <si>
+    <t>First File Offset</t>
+  </si>
+  <si>
+    <t>ALB byte Size</t>
+  </si>
+  <si>
+    <t>File ALB</t>
+  </si>
+  <si>
+    <t>File Offset</t>
   </si>
 </sst>
 </file>
@@ -941,7 +990,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -997,19 +1046,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1019,12 +1061,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1037,9 +1078,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1050,16 +1088,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1079,9 +1119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1119,7 +1159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1225,7 +1265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1367,7 +1407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4007,7 +4047,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1429739E-2066-4D15-810F-4CE51F2F0E14}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
@@ -4020,7 +4060,7 @@
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>73</v>
       </c>
@@ -4040,7 +4080,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -4058,16 +4098,10 @@
       </c>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -4075,11 +4109,11 @@
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -4091,11 +4125,11 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -4107,20 +4141,14 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -4136,11 +4164,11 @@
       <c r="E8" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -4156,20 +4184,14 @@
       <c r="E9" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4182,21 +4204,21 @@
       <c r="D11" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>133</v>
       </c>
@@ -4245,12 +4267,7 @@
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -4260,7 +4277,7 @@
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
-      <c r="F22" s="23"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -4270,7 +4287,7 @@
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
-      <c r="F23" s="23"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -4280,15 +4297,10 @@
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="23"/>
+      <c r="F24" s="20"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -4302,7 +4314,7 @@
         <v>214</v>
       </c>
       <c r="E26" s="20"/>
-      <c r="F26" s="23"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -4312,15 +4324,10 @@
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="23"/>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+      <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -4331,8 +4338,8 @@
       <c r="D29" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -4343,8 +4350,8 @@
       <c r="D30" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -4355,8 +4362,8 @@
       <c r="D31" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -4367,8 +4374,8 @@
       <c r="D32" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -4379,15 +4386,15 @@
       <c r="D33" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
@@ -4404,8 +4411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F62009-2B4D-46CE-8D10-92156B101088}">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N31" sqref="N29:N31"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4420,27 +4427,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="32" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="33" t="s">
         <v>98</v>
       </c>
       <c r="H2" s="17" t="s">
@@ -4458,7 +4465,7 @@
       <c r="A3" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="31">
         <v>16</v>
       </c>
       <c r="C3">
@@ -4482,44 +4489,44 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
+      <c r="B4" s="31"/>
       <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
+      <c r="B5" s="31"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
+      <c r="B6" s="31"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="35"/>
+      <c r="B7" s="31"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>147</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="G8" s="36"/>
+      <c r="G8" s="32"/>
       <c r="H8" s="17" t="s">
         <v>140</v>
       </c>
@@ -4628,22 +4635,22 @@
       <c r="A15" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="36"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="17" t="s">
         <v>140</v>
       </c>
@@ -4654,7 +4661,7 @@
         <v>142</v>
       </c>
       <c r="K15" s="17"/>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="33" t="s">
         <v>145</v>
       </c>
       <c r="M15">
@@ -4777,29 +4784,29 @@
       <c r="A22" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="31"/>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>177</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="E23" s="37" t="s">
+      <c r="E23" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="36"/>
+      <c r="G23" s="32"/>
       <c r="H23" s="17" t="s">
         <v>140</v>
       </c>
@@ -4844,29 +4851,29 @@
       <c r="A27" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="31"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>177</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="E28" s="37" t="s">
+      <c r="E28" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="G28" s="36"/>
+      <c r="G28" s="32"/>
       <c r="H28" s="17" t="s">
         <v>140</v>
       </c>
@@ -4900,7 +4907,7 @@
         <f>B29*C29*D29*E29</f>
         <v>102400</v>
       </c>
-      <c r="H29" s="38" t="s">
+      <c r="H29" s="34" t="s">
         <v>180</v>
       </c>
       <c r="I29">
@@ -4943,7 +4950,7 @@
       <c r="A32" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="31"/>
       <c r="F32" s="11"/>
       <c r="H32" s="8"/>
     </row>
@@ -4951,22 +4958,22 @@
       <c r="A33" t="s">
         <v>177</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="37" t="s">
+      <c r="D33" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="E33" s="37" t="s">
+      <c r="E33" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F33" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="G33" s="36"/>
+      <c r="G33" s="32"/>
       <c r="H33" s="17" t="s">
         <v>140</v>
       </c>
@@ -4997,7 +5004,7 @@
         <f>B34*C34*D34*E34</f>
         <v>102400</v>
       </c>
-      <c r="H34" s="38" t="s">
+      <c r="H34" s="34" t="s">
         <v>180</v>
       </c>
       <c r="I34">
@@ -5015,10 +5022,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B79399-9BB6-4B97-BE36-8FE45530B141}">
-  <dimension ref="A2:AO46"/>
+  <dimension ref="A2:AO49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N6" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5111,31 +5118,31 @@
       <c r="P6" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="S6" s="28" t="s">
+      <c r="S6" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="T6" s="28" t="s">
+      <c r="T6" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="U6" s="28" t="s">
+      <c r="U6" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="V6" s="28" t="s">
+      <c r="V6" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="W6" s="28" t="s">
+      <c r="W6" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="X6" s="28" t="s">
+      <c r="X6" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="Y6" s="29" t="s">
+      <c r="Y6" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="Z6" s="29" t="s">
+      <c r="Z6" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AA6" s="29" t="s">
+      <c r="AA6" s="26" t="s">
         <v>120</v>
       </c>
       <c r="AB6" s="7" t="s">
@@ -5209,30 +5216,30 @@
         <f>O7/(I7*H7)</f>
         <v>2</v>
       </c>
-      <c r="S7" s="30" t="s">
+      <c r="S7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="T7" s="30">
+      <c r="T7" s="27">
         <v>18</v>
       </c>
-      <c r="U7" s="30">
+      <c r="U7" s="27">
         <v>512</v>
       </c>
-      <c r="V7" s="31">
+      <c r="V7" s="28">
         <v>80</v>
       </c>
-      <c r="W7" s="30">
+      <c r="W7" s="27">
         <v>2</v>
       </c>
-      <c r="X7" s="32">
+      <c r="X7" s="29">
         <f>T7*U7*V7*W7</f>
         <v>1474560</v>
       </c>
-      <c r="Y7" s="33"/>
-      <c r="Z7" s="33" t="s">
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="AA7" s="33" t="s">
+      <c r="AA7" s="30" t="s">
         <v>3</v>
       </c>
       <c r="AB7" s="7">
@@ -5241,11 +5248,11 @@
       <c r="AC7" s="7">
         <v>2048</v>
       </c>
-      <c r="AD7" s="42">
+      <c r="AD7" s="37">
         <f>X7/AC7</f>
         <v>720</v>
       </c>
-      <c r="AE7" s="42"/>
+      <c r="AE7" s="37"/>
       <c r="AF7" s="7">
         <v>8192</v>
       </c>
@@ -5308,32 +5315,32 @@
         <f t="shared" ref="P8:P13" si="0">O8/(I8*H8)</f>
         <v>1.8</v>
       </c>
-      <c r="S8" s="31" t="s">
+      <c r="S8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="T8" s="31">
+      <c r="T8" s="28">
         <v>5</v>
       </c>
-      <c r="U8" s="31">
+      <c r="U8" s="28">
         <v>1024</v>
       </c>
-      <c r="V8" s="31">
+      <c r="V8" s="28">
         <v>80</v>
       </c>
-      <c r="W8" s="31">
+      <c r="W8" s="28">
         <v>2</v>
       </c>
-      <c r="X8" s="43">
+      <c r="X8" s="38">
         <f t="shared" ref="X8:X18" si="1">T8*U8*V8*W8</f>
         <v>819200</v>
       </c>
       <c r="Y8" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="Z8" s="33" t="s">
+      <c r="Z8" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="AA8" s="33" t="s">
+      <c r="AA8" s="30" t="s">
         <v>3</v>
       </c>
       <c r="AB8" s="7">
@@ -5342,25 +5349,25 @@
       <c r="AC8" s="7">
         <v>2048</v>
       </c>
-      <c r="AD8" s="42">
+      <c r="AD8" s="37">
         <f t="shared" ref="AD8:AD17" si="2">X8/AC8</f>
         <v>400</v>
       </c>
-      <c r="AE8" s="42">
+      <c r="AE8" s="37">
         <v>394</v>
       </c>
       <c r="AF8" s="7">
         <v>8192</v>
       </c>
-      <c r="AI8" s="40">
+      <c r="AI8" s="36">
         <f>AC8*(AE8+1)</f>
         <v>808960</v>
       </c>
-      <c r="AJ8" s="40">
+      <c r="AJ8" s="36">
         <f>AI8+AB8</f>
         <v>819200</v>
       </c>
-      <c r="AK8" s="40"/>
+      <c r="AK8" s="36"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
@@ -5413,32 +5420,32 @@
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="S9" s="31" t="s">
+      <c r="S9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="T9" s="31">
+      <c r="T9" s="28">
         <v>16</v>
       </c>
-      <c r="U9" s="31">
+      <c r="U9" s="28">
         <v>256</v>
       </c>
-      <c r="V9" s="31">
+      <c r="V9" s="28">
         <v>80</v>
       </c>
-      <c r="W9" s="31">
+      <c r="W9" s="28">
         <v>2</v>
       </c>
-      <c r="X9" s="43">
+      <c r="X9" s="38">
         <f t="shared" si="1"/>
         <v>655360</v>
       </c>
       <c r="Y9" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="Z9" s="33" t="s">
+      <c r="Z9" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="AA9" s="33" t="s">
+      <c r="AA9" s="30" t="s">
         <v>3</v>
       </c>
       <c r="AB9" s="7">
@@ -5447,11 +5454,11 @@
       <c r="AC9" s="7">
         <v>2048</v>
       </c>
-      <c r="AD9" s="42">
+      <c r="AD9" s="37">
         <f t="shared" si="2"/>
         <v>320</v>
       </c>
-      <c r="AE9" s="42"/>
+      <c r="AE9" s="37"/>
       <c r="AF9" s="7">
         <v>8192</v>
       </c>
@@ -5508,32 +5515,32 @@
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="S10" s="31" t="s">
+      <c r="S10" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="T10" s="31">
+      <c r="T10" s="28">
         <v>5</v>
       </c>
-      <c r="U10" s="31">
+      <c r="U10" s="28">
         <v>1024</v>
       </c>
-      <c r="V10" s="31">
+      <c r="V10" s="28">
         <v>40</v>
       </c>
-      <c r="W10" s="31">
+      <c r="W10" s="28">
         <v>2</v>
       </c>
-      <c r="X10" s="32">
+      <c r="X10" s="29">
         <f t="shared" si="1"/>
         <v>409600</v>
       </c>
       <c r="Y10" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="Z10" s="33" t="s">
+      <c r="Z10" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="AA10" s="33" t="s">
+      <c r="AA10" s="30" t="s">
         <v>3</v>
       </c>
       <c r="AB10" s="7">
@@ -5542,28 +5549,28 @@
       <c r="AC10" s="7">
         <v>2048</v>
       </c>
-      <c r="AD10" s="42">
+      <c r="AD10" s="37">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="AE10" s="42">
+      <c r="AE10" s="37">
         <v>194</v>
       </c>
       <c r="AF10" s="7">
         <v>4096</v>
       </c>
-      <c r="AG10" s="41">
+      <c r="AG10" s="7">
         <v>4</v>
       </c>
       <c r="AH10" t="str">
         <f>DEC2HEX(AB10+AC10*AG10)</f>
         <v>4800</v>
       </c>
-      <c r="AI10" s="40">
+      <c r="AI10" s="36">
         <f>AC10*(AE10+1)</f>
         <v>399360</v>
       </c>
-      <c r="AJ10" s="40">
+      <c r="AJ10" s="36">
         <f>AI10+AB10</f>
         <v>409600</v>
       </c>
@@ -5619,32 +5626,32 @@
         <f t="shared" si="0"/>
         <v>1.125</v>
       </c>
-      <c r="S11" s="34" t="s">
+      <c r="S11" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="T11" s="31">
+      <c r="T11" s="28">
         <v>16</v>
       </c>
-      <c r="U11" s="31">
+      <c r="U11" s="28">
         <v>256</v>
       </c>
-      <c r="V11" s="31">
+      <c r="V11" s="28">
         <v>40</v>
       </c>
-      <c r="W11" s="31">
+      <c r="W11" s="28">
         <v>1</v>
       </c>
-      <c r="X11" s="32">
+      <c r="X11" s="29">
         <f t="shared" si="1"/>
         <v>163840</v>
       </c>
       <c r="Y11" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="Z11" s="33" t="s">
+      <c r="Z11" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="AA11" s="33" t="s">
+      <c r="AA11" s="30" t="s">
         <v>3</v>
       </c>
       <c r="AB11" s="7">
@@ -5653,18 +5660,18 @@
       <c r="AC11" s="7">
         <v>2048</v>
       </c>
-      <c r="AD11" s="42">
+      <c r="AD11" s="37">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="AE11" s="42"/>
+      <c r="AE11" s="37"/>
       <c r="AF11" s="7">
         <v>2048</v>
       </c>
-      <c r="AG11" s="41"/>
-      <c r="AI11" s="40"/>
-      <c r="AJ11" s="40"/>
-      <c r="AK11" s="40"/>
+      <c r="AG11" s="7"/>
+      <c r="AI11" s="36"/>
+      <c r="AJ11" s="36"/>
+      <c r="AK11" s="36"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
@@ -5720,32 +5727,32 @@
       <c r="R12" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="31" t="s">
+      <c r="S12" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="T12" s="31">
+      <c r="T12" s="28">
         <v>8</v>
       </c>
-      <c r="U12" s="31">
+      <c r="U12" s="28">
         <v>512</v>
       </c>
-      <c r="V12" s="31">
+      <c r="V12" s="28">
         <v>40</v>
       </c>
-      <c r="W12" s="31">
+      <c r="W12" s="28">
         <v>2</v>
       </c>
-      <c r="X12" s="32">
+      <c r="X12" s="29">
         <f t="shared" si="1"/>
         <v>327680</v>
       </c>
       <c r="Y12" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="Z12" s="33" t="s">
+      <c r="Z12" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="AA12" s="33" t="s">
+      <c r="AA12" s="30" t="s">
         <v>3</v>
       </c>
       <c r="AB12" s="7">
@@ -5754,32 +5761,32 @@
       <c r="AC12" s="7">
         <v>2048</v>
       </c>
-      <c r="AD12" s="42">
+      <c r="AD12" s="37">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="AE12" s="42">
+      <c r="AE12" s="37">
         <v>155</v>
       </c>
       <c r="AF12" s="7">
         <v>8192</v>
       </c>
-      <c r="AG12" s="41">
+      <c r="AG12" s="7">
         <v>4</v>
       </c>
       <c r="AH12" t="str">
         <f t="shared" ref="AH12:AH16" si="4">DEC2HEX(AB12+AC12*AG12)</f>
         <v>4000</v>
       </c>
-      <c r="AI12" s="40">
+      <c r="AI12" s="36">
         <f>AC12*(AE12+1)</f>
         <v>319488</v>
       </c>
-      <c r="AJ12" s="40">
+      <c r="AJ12" s="36">
         <f>AI12+AB12</f>
         <v>327680</v>
       </c>
-      <c r="AL12" s="41">
+      <c r="AL12" s="7">
         <v>16</v>
       </c>
       <c r="AM12">
@@ -5845,32 +5852,32 @@
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="S13" s="31" t="s">
+      <c r="S13" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="T13" s="31">
+      <c r="T13" s="28">
         <v>10</v>
       </c>
-      <c r="U13" s="31">
+      <c r="U13" s="28">
         <v>256</v>
       </c>
-      <c r="V13" s="31">
+      <c r="V13" s="28">
         <v>40</v>
       </c>
-      <c r="W13" s="31">
+      <c r="W13" s="28">
         <v>1</v>
       </c>
-      <c r="X13" s="32">
+      <c r="X13" s="29">
         <f t="shared" si="1"/>
         <v>102400</v>
       </c>
       <c r="Y13" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="Z13" s="33" t="s">
+      <c r="Z13" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="AA13" s="33" t="s">
+      <c r="AA13" s="30" t="s">
         <v>3</v>
       </c>
       <c r="AB13" s="7">
@@ -5879,11 +5886,11 @@
       <c r="AC13" s="7">
         <v>1024</v>
       </c>
-      <c r="AD13" s="42">
+      <c r="AD13" s="37">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="AE13" s="42"/>
+      <c r="AE13" s="37"/>
       <c r="AF13" s="7">
         <v>2048</v>
       </c>
@@ -5933,30 +5940,30 @@
       <c r="M14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="S14" s="31" t="s">
+      <c r="S14" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="T14" s="31">
+      <c r="T14" s="28">
         <v>10</v>
       </c>
-      <c r="U14" s="31">
+      <c r="U14" s="28">
         <v>256</v>
       </c>
-      <c r="V14" s="31">
+      <c r="V14" s="28">
         <v>40</v>
       </c>
-      <c r="W14" s="31">
+      <c r="W14" s="28">
         <v>1</v>
       </c>
-      <c r="X14" s="32">
+      <c r="X14" s="29">
         <f t="shared" si="1"/>
         <v>102400</v>
       </c>
       <c r="Y14" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="Z14" s="31"/>
-      <c r="AA14" s="33" t="s">
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="30" t="s">
         <v>3</v>
       </c>
       <c r="AB14" s="7">
@@ -5965,11 +5972,11 @@
       <c r="AC14" s="7">
         <v>1024</v>
       </c>
-      <c r="AD14" s="42">
+      <c r="AD14" s="37">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="AE14" s="42"/>
+      <c r="AE14" s="37"/>
       <c r="AF14" s="7">
         <v>2048</v>
       </c>
@@ -6019,30 +6026,30 @@
       <c r="M15" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="S15" s="31" t="s">
+      <c r="S15" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="T15" s="31">
+      <c r="T15" s="28">
         <v>10</v>
       </c>
-      <c r="U15" s="31">
+      <c r="U15" s="28">
         <v>256</v>
       </c>
-      <c r="V15" s="31">
+      <c r="V15" s="28">
         <v>40</v>
       </c>
-      <c r="W15" s="31">
+      <c r="W15" s="28">
         <v>1</v>
       </c>
-      <c r="X15" s="32">
+      <c r="X15" s="29">
         <f t="shared" si="1"/>
         <v>102400</v>
       </c>
       <c r="Y15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="Z15" s="31"/>
-      <c r="AA15" s="33" t="s">
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="30" t="s">
         <v>3</v>
       </c>
       <c r="AB15" s="7">
@@ -6051,11 +6058,11 @@
       <c r="AC15" s="7">
         <v>1024</v>
       </c>
-      <c r="AD15" s="42">
+      <c r="AD15" s="37">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="AE15" s="42"/>
+      <c r="AE15" s="37"/>
       <c r="AF15" s="7">
         <v>2048</v>
       </c>
@@ -6066,41 +6073,41 @@
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="S16" s="34" t="s">
+      <c r="S16" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="T16" s="34">
+      <c r="T16" s="28">
         <v>8</v>
       </c>
-      <c r="U16" s="34">
+      <c r="U16" s="28">
         <v>512</v>
       </c>
-      <c r="V16" s="34">
+      <c r="V16" s="28">
         <v>40</v>
       </c>
-      <c r="W16" s="34">
+      <c r="W16" s="28">
         <v>2</v>
       </c>
-      <c r="X16" s="32">
+      <c r="X16" s="29">
         <f t="shared" si="1"/>
         <v>327680</v>
       </c>
       <c r="Y16" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="Z16" s="31"/>
-      <c r="AA16" s="33"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="30"/>
       <c r="AB16" s="7">
         <v>8192</v>
       </c>
       <c r="AC16">
         <v>2048</v>
       </c>
-      <c r="AD16" s="42">
+      <c r="AD16" s="37">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="AE16" s="42">
+      <c r="AE16" s="37">
         <v>155</v>
       </c>
       <c r="AF16" s="7">
@@ -6113,759 +6120,780 @@
         <f t="shared" si="4"/>
         <v>5800</v>
       </c>
-      <c r="AI16" s="40">
+      <c r="AI16" s="36">
         <f>AC16*(AE16+1)</f>
         <v>319488</v>
       </c>
-      <c r="AJ16" s="40">
+      <c r="AJ16" s="36">
         <f>AI16+AB16</f>
         <v>327680</v>
       </c>
-      <c r="AK16" s="40"/>
+      <c r="AK16" s="36"/>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
+      <c r="B17" t="s">
+        <v>251</v>
+      </c>
       <c r="R17" t="s">
         <v>250</v>
       </c>
-      <c r="S17" s="46"/>
-      <c r="T17" s="51">
+      <c r="T17" s="43">
         <v>10</v>
       </c>
-      <c r="U17" s="51">
+      <c r="U17" s="43">
         <v>256</v>
       </c>
-      <c r="V17" s="51">
+      <c r="V17" s="43">
         <v>40</v>
       </c>
-      <c r="W17" s="51">
+      <c r="W17" s="43">
         <v>2</v>
       </c>
-      <c r="X17" s="47">
+      <c r="X17" s="41">
         <f t="shared" si="1"/>
         <v>204800</v>
       </c>
-      <c r="Y17" s="48"/>
-      <c r="Z17" s="49"/>
-      <c r="AA17" s="50"/>
+      <c r="Y17" s="8"/>
+      <c r="AA17" s="42"/>
       <c r="AB17" s="7">
         <v>7680</v>
       </c>
       <c r="AC17" s="7">
         <v>2048</v>
       </c>
-      <c r="AD17" s="42">
+      <c r="AD17" s="37">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="AE17" s="42"/>
+      <c r="AE17" s="37"/>
       <c r="AF17" s="7">
         <v>8192</v>
       </c>
-      <c r="AI17" s="40"/>
-      <c r="AJ17" s="40"/>
-      <c r="AK17" s="40"/>
+      <c r="AI17" s="36"/>
+      <c r="AJ17" s="36"/>
+      <c r="AK17" s="36"/>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="R18" t="s">
         <v>250</v>
       </c>
-      <c r="S18" s="46"/>
-      <c r="T18" s="51">
+      <c r="T18" s="43">
         <v>10</v>
       </c>
-      <c r="U18" s="51">
+      <c r="U18" s="43">
         <v>256</v>
       </c>
-      <c r="V18" s="51">
+      <c r="V18" s="43">
         <v>80</v>
       </c>
-      <c r="W18" s="51">
+      <c r="W18" s="43">
         <v>2</v>
       </c>
-      <c r="X18" s="47">
+      <c r="X18" s="41">
         <f t="shared" si="1"/>
         <v>409600</v>
       </c>
-      <c r="Y18" s="48"/>
-      <c r="Z18" s="49"/>
-      <c r="AA18" s="50"/>
+      <c r="Y18" s="8"/>
+      <c r="AA18" s="42"/>
       <c r="AB18" s="7">
         <v>7680</v>
       </c>
       <c r="AC18" s="7">
         <v>2048</v>
       </c>
-      <c r="AD18" s="42">
+      <c r="AD18" s="37">
         <f t="shared" ref="AD18" si="5">X18/AC18</f>
         <v>200</v>
       </c>
-      <c r="AE18" s="42"/>
+      <c r="AE18" s="37"/>
       <c r="AF18" s="7">
         <v>8192</v>
       </c>
-      <c r="AI18" s="40"/>
-      <c r="AJ18" s="40"/>
-      <c r="AK18" s="40"/>
+      <c r="AI18" s="36"/>
+      <c r="AJ18" s="36"/>
+      <c r="AK18" s="36"/>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
-      <c r="S19" s="46"/>
-      <c r="T19" s="46"/>
-      <c r="U19" s="46"/>
-      <c r="V19" s="46"/>
-      <c r="W19" s="46"/>
-      <c r="X19" s="47"/>
-      <c r="Y19" s="48"/>
-      <c r="Z19" s="49"/>
-      <c r="AA19" s="50"/>
+      <c r="N19" s="8"/>
+      <c r="T19" s="44"/>
+      <c r="U19" s="44"/>
+      <c r="V19" s="44"/>
+      <c r="W19" s="44"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="8"/>
+      <c r="AA19" s="42"/>
       <c r="AB19" s="7"/>
-      <c r="AD19" s="42"/>
-      <c r="AE19" s="42"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="37"/>
+      <c r="AE19" s="37"/>
       <c r="AF19" s="7"/>
-      <c r="AI19" s="40"/>
-      <c r="AJ19" s="40"/>
-      <c r="AK19" s="40"/>
+      <c r="AI19" s="36"/>
+      <c r="AJ19" s="36"/>
+      <c r="AK19" s="36"/>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
+      <c r="T20" s="44"/>
+      <c r="U20" s="44"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="44"/>
+      <c r="X20" s="41"/>
       <c r="Y20" s="8"/>
-    </row>
-    <row r="21" spans="1:38" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="AA20" s="42"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="37"/>
+      <c r="AE20" s="37"/>
+      <c r="AF20" s="7"/>
+      <c r="AI20" s="36"/>
+      <c r="AJ20" s="36"/>
+      <c r="AK20" s="36"/>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="44"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="8"/>
+      <c r="AA21" s="42"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="37"/>
+      <c r="AE21" s="37"/>
+      <c r="AF21" s="7"/>
+      <c r="AI21" s="36"/>
+      <c r="AJ21" s="36"/>
+      <c r="AK21" s="36"/>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="8"/>
+      <c r="AA22" s="42"/>
+      <c r="AB22" s="7"/>
+      <c r="AD22" s="37"/>
+      <c r="AE22" s="37"/>
+      <c r="AF22" s="7"/>
+      <c r="AI22" s="36"/>
+      <c r="AJ22" s="36"/>
+      <c r="AK22" s="36"/>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="Y23" s="8"/>
+    </row>
+    <row r="24" spans="1:38" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="I24" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J24" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="K24" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="L24" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="M21" s="7" t="s">
+      <c r="M24" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="N21" s="14" t="s">
+      <c r="N24" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="O21" s="7" t="s">
+      <c r="O24" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="P21" s="7" t="s">
+      <c r="P24" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="Q21" s="14"/>
-      <c r="T21" s="16" t="s">
+      <c r="Q24" s="14"/>
+      <c r="T24" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="U21" s="16" t="s">
+      <c r="U24" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="V21" s="16" t="s">
+      <c r="V24" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="W21" s="16" t="s">
+      <c r="W24" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="X21" s="16" t="s">
+      <c r="X24" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="Y21" s="16" t="s">
+      <c r="Y24" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="Z21" s="17" t="s">
+      <c r="Z24" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="AA21" s="17" t="s">
+      <c r="AA24" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
         <v>0</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>102</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>33</v>
       </c>
-      <c r="E22">
+      <c r="E25">
         <v>1</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F25" t="s">
         <v>22</v>
       </c>
-      <c r="G22">
+      <c r="G25">
         <v>1</v>
       </c>
-      <c r="H22">
+      <c r="H25">
         <v>8</v>
       </c>
-      <c r="I22">
+      <c r="I25">
         <v>512</v>
       </c>
-      <c r="J22">
+      <c r="J25">
         <v>40</v>
       </c>
-      <c r="K22">
+      <c r="K25">
         <v>2</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L25" t="s">
         <v>107</v>
       </c>
-      <c r="M22">
+      <c r="M25">
         <v>1</v>
       </c>
-      <c r="N22" s="8" t="s">
+      <c r="N25" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O25" t="s">
         <v>112</v>
       </c>
-      <c r="P22" s="11">
-        <f>H22*I22*J22*K22</f>
+      <c r="P25" s="11">
+        <f>H25*I25*J25*K25</f>
         <v>327680</v>
       </c>
-      <c r="Q22" s="8" t="s">
+      <c r="Q25" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="T22" s="31" t="s">
+      <c r="T25" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="U22" s="31">
+      <c r="U25" s="28">
         <v>8</v>
       </c>
-      <c r="V22" s="31">
+      <c r="V25" s="28">
         <v>512</v>
       </c>
-      <c r="W22" s="31">
+      <c r="W25" s="28">
         <v>40</v>
       </c>
-      <c r="X22" s="31">
+      <c r="X25" s="28">
         <v>2</v>
       </c>
-      <c r="Y22" s="32">
-        <f t="shared" ref="Y22:Y25" si="6">U22*V22*W22*X22</f>
+      <c r="Y25" s="29">
+        <f t="shared" ref="Y25:Y28" si="6">U25*V25*W25*X25</f>
         <v>327680</v>
       </c>
-      <c r="Z22" s="18" t="s">
+      <c r="Z25" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AA22" s="33" t="s">
+      <c r="AA25" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="AG22">
+      <c r="AG25">
         <f>9*512</f>
         <v>4608</v>
       </c>
-      <c r="AH22" t="str">
-        <f>DEC2HEX(AG22)</f>
+      <c r="AH25" t="str">
+        <f>DEC2HEX(AG25)</f>
         <v>1200</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
         <v>1</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>103</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>27</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>33</v>
       </c>
-      <c r="E23">
+      <c r="E26">
         <v>1</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F26" t="s">
         <v>22</v>
       </c>
-      <c r="G23">
+      <c r="G26">
         <v>1</v>
       </c>
-      <c r="H23">
+      <c r="H26">
         <v>9</v>
       </c>
-      <c r="I23">
+      <c r="I26">
         <v>512</v>
       </c>
-      <c r="J23">
+      <c r="J26">
         <v>40</v>
       </c>
-      <c r="K23">
+      <c r="K26">
         <v>2</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L26" t="s">
         <v>107</v>
       </c>
-      <c r="M23">
+      <c r="M26">
         <v>2</v>
       </c>
-      <c r="N23" s="8" t="s">
+      <c r="N26" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O26" t="s">
         <v>113</v>
       </c>
-      <c r="P23" s="11">
-        <f t="shared" ref="P23:P25" si="7">H23*I23*J23*K23</f>
+      <c r="P26" s="11">
+        <f t="shared" ref="P26:P28" si="7">H26*I26*J26*K26</f>
         <v>368640</v>
       </c>
-      <c r="Q23" s="8" t="s">
+      <c r="Q26" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="T23" s="31" t="s">
+      <c r="T26" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="U23" s="31">
+      <c r="U26" s="28">
         <v>9</v>
       </c>
-      <c r="V23" s="31">
+      <c r="V26" s="28">
         <v>512</v>
       </c>
-      <c r="W23" s="31">
+      <c r="W26" s="28">
         <v>40</v>
       </c>
-      <c r="X23" s="31">
+      <c r="X26" s="28">
         <v>2</v>
       </c>
-      <c r="Y23" s="32">
+      <c r="Y26" s="29">
         <f t="shared" si="6"/>
         <v>368640</v>
       </c>
-      <c r="Z23" s="18" t="s">
+      <c r="Z26" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AA23" s="33" t="s">
+      <c r="AA26" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="AG23">
-        <f>AG$22+AG22</f>
+      <c r="AG26">
+        <f>AG$25+AG25</f>
         <v>9216</v>
       </c>
-      <c r="AH23" t="str">
-        <f>DEC2HEX(AG23)</f>
+      <c r="AH26" t="str">
+        <f>DEC2HEX(AG26)</f>
         <v>2400</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
         <v>2</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>104</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>27</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="E24">
+      <c r="E27">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F27" t="s">
         <v>22</v>
       </c>
-      <c r="G24">
+      <c r="G27">
         <v>1</v>
       </c>
-      <c r="H24">
+      <c r="H27">
         <v>8</v>
       </c>
-      <c r="I24">
+      <c r="I27">
         <v>512</v>
       </c>
-      <c r="J24">
+      <c r="J27">
         <v>80</v>
       </c>
-      <c r="K24">
+      <c r="K27">
         <v>2</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L27" t="s">
         <v>107</v>
       </c>
-      <c r="M24">
+      <c r="M27">
         <v>2</v>
       </c>
-      <c r="N24" s="8" t="s">
+      <c r="N27" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O27" t="s">
         <v>115</v>
       </c>
-      <c r="P24" s="11">
+      <c r="P27" s="11">
         <f t="shared" si="7"/>
         <v>655360</v>
       </c>
-      <c r="Q24" s="8" t="s">
+      <c r="Q27" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="T24" s="31" t="s">
+      <c r="T27" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="U24" s="31">
+      <c r="U27" s="28">
         <v>8</v>
       </c>
-      <c r="V24" s="31">
+      <c r="V27" s="28">
         <v>512</v>
       </c>
-      <c r="W24" s="31">
+      <c r="W27" s="28">
         <v>80</v>
       </c>
-      <c r="X24" s="31">
+      <c r="X27" s="28">
         <v>2</v>
       </c>
-      <c r="Y24" s="32">
+      <c r="Y27" s="29">
         <f t="shared" si="6"/>
         <v>655360</v>
       </c>
-      <c r="Z24" s="18" t="s">
+      <c r="Z27" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AA24" s="33" t="s">
+      <c r="AA27" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="AG24">
-        <f>AG$22+AG23</f>
+      <c r="AG27">
+        <f>AG$25+AG26</f>
         <v>13824</v>
       </c>
-      <c r="AH24" t="str">
-        <f>DEC2HEX(AG24)</f>
+      <c r="AH27" t="str">
+        <f>DEC2HEX(AG27)</f>
         <v>3600</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
         <v>3</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>105</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>27</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>106</v>
       </c>
-      <c r="E25">
+      <c r="E28">
         <v>1</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F28" t="s">
         <v>22</v>
       </c>
-      <c r="G25">
+      <c r="G28">
         <v>1</v>
       </c>
-      <c r="H25">
+      <c r="H28">
         <v>8</v>
       </c>
-      <c r="I25">
+      <c r="I28">
         <v>1024</v>
       </c>
-      <c r="J25">
+      <c r="J28">
         <v>77</v>
       </c>
-      <c r="K25">
+      <c r="K28">
         <v>2</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L28" t="s">
         <v>108</v>
       </c>
-      <c r="M25">
+      <c r="M28">
         <v>2</v>
       </c>
-      <c r="N25" s="8" t="s">
+      <c r="N28" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O28" t="s">
         <v>114</v>
       </c>
-      <c r="P25" s="11">
+      <c r="P28" s="11">
         <f t="shared" si="7"/>
         <v>1261568</v>
       </c>
-      <c r="Q25" s="8" t="s">
+      <c r="Q28" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="T25" s="31" t="s">
+      <c r="T28" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="U25" s="31">
+      <c r="U28" s="28">
         <v>8</v>
       </c>
-      <c r="V25" s="31">
+      <c r="V28" s="28">
         <v>1024</v>
       </c>
-      <c r="W25" s="31">
+      <c r="W28" s="28">
         <v>77</v>
       </c>
-      <c r="X25" s="31">
+      <c r="X28" s="28">
         <v>2</v>
       </c>
-      <c r="Y25" s="32">
+      <c r="Y28" s="29">
         <f t="shared" si="6"/>
         <v>1261568</v>
       </c>
-      <c r="Z25" s="18" t="s">
+      <c r="Z28" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AA25" s="33" t="s">
+      <c r="AA28" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="AG25">
-        <f>AG$22+AG24</f>
+      <c r="AG28">
+        <f>AG$25+AG27</f>
         <v>18432</v>
       </c>
-      <c r="AH25" t="str">
-        <f>DEC2HEX(AG25)</f>
+      <c r="AH28" t="str">
+        <f>DEC2HEX(AG28)</f>
         <v>4800</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="H26">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H29">
         <v>18</v>
       </c>
-      <c r="I26">
+      <c r="I29">
         <v>512</v>
       </c>
-      <c r="J26">
+      <c r="J29">
         <v>80</v>
       </c>
-      <c r="K26">
+      <c r="K29">
         <v>2</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L29" t="s">
         <v>107</v>
       </c>
-      <c r="M26">
+      <c r="M29">
         <v>9</v>
       </c>
-      <c r="N26" s="8" t="s">
+      <c r="N29" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O29" t="s">
         <v>174</v>
       </c>
-      <c r="P26" s="11">
-        <f>H26*I26*J26*K26</f>
+      <c r="P29" s="11">
+        <f>H29*I29*J29*K29</f>
         <v>1474560</v>
       </c>
-      <c r="Q26" s="8" t="s">
+      <c r="Q29" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="T26" s="31" t="s">
+      <c r="T29" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="U26" s="31">
+      <c r="U29" s="28">
         <v>18</v>
       </c>
-      <c r="V26" s="31">
+      <c r="V29" s="28">
         <v>512</v>
       </c>
-      <c r="W26" s="31">
+      <c r="W29" s="28">
         <v>80</v>
       </c>
-      <c r="X26" s="31">
+      <c r="X29" s="28">
         <v>2</v>
       </c>
-      <c r="Y26" s="32">
-        <f t="shared" ref="Y26" si="8">U26*V26*W26*X26</f>
+      <c r="Y29" s="29">
+        <f t="shared" ref="Y29" si="8">U29*V29*W29*X29</f>
         <v>1474560</v>
       </c>
-      <c r="Z26" s="18" t="s">
+      <c r="Z29" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AA26" s="33" t="s">
+      <c r="AA29" s="30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ27" t="s">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AJ30" t="s">
         <v>223</v>
       </c>
-      <c r="AK27" t="s">
+      <c r="AK30" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AH28" t="s">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AH31" t="s">
         <v>239</v>
       </c>
-      <c r="AI28" t="s">
+      <c r="AI31" t="s">
         <v>240</v>
       </c>
-      <c r="AJ28" t="s">
+      <c r="AJ31" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AH29">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AH32">
         <v>72</v>
       </c>
-      <c r="AI29" s="8">
+      <c r="AI32" s="8">
         <v>48</v>
       </c>
-      <c r="AJ29" s="44">
+      <c r="AJ32" s="39">
         <v>20</v>
       </c>
-      <c r="AK29">
+      <c r="AK32">
         <v>32</v>
       </c>
-      <c r="AL29" t="s">
+      <c r="AL32" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI30" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ30" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI31" s="8">
-        <v>5</v>
-      </c>
-      <c r="AJ31" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI32" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="AJ32" s="8" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="33" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI33" s="8">
         <v>0</v>
       </c>
-      <c r="AJ33" s="8">
+      <c r="AJ33" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI34" s="8">
+        <v>5</v>
+      </c>
+      <c r="AJ34" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI35" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ35" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="36" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI36" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI34" s="8" t="s">
+    <row r="37" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI37" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="AJ34" s="44" t="s">
+      <c r="AJ37" s="39" t="s">
         <v>243</v>
       </c>
-      <c r="AK34">
+      <c r="AK37">
         <v>155</v>
       </c>
-      <c r="AL34" t="s">
+      <c r="AL37" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI35" s="8">
+    <row r="38" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI38" s="8">
         <v>6</v>
       </c>
-      <c r="AJ35" s="45">
+      <c r="AJ38" s="40">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI36" s="8" t="s">
+    <row r="39" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI39" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AJ36" s="44" t="s">
+      <c r="AJ39" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="AK36">
+      <c r="AK39">
         <v>255</v>
       </c>
-      <c r="AL36" t="s">
+      <c r="AL39" t="s">
         <v>247</v>
-      </c>
-    </row>
-    <row r="37" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI37" s="8">
-        <v>3</v>
-      </c>
-      <c r="AJ37" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI38" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ38" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI39" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ39" s="8">
-        <v>0</v>
       </c>
     </row>
     <row r="40" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI40" s="8">
+        <v>3</v>
+      </c>
+      <c r="AJ40" s="40">
         <v>0</v>
       </c>
-      <c r="AJ40" s="8">
-        <v>40</v>
-      </c>
     </row>
     <row r="41" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI41" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ41" s="8">
-        <v>0</v>
+      <c r="AI41" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ41" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI42" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ42" s="8">
-        <v>2</v>
-      </c>
-      <c r="AL42" t="s">
-        <v>248</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="35:38" x14ac:dyDescent="0.25">
@@ -6873,20 +6901,47 @@
         <v>0</v>
       </c>
       <c r="AJ43" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI44" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI44" s="8"/>
-      <c r="AJ44" s="8"/>
+      <c r="AJ44" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI45" s="8"/>
-      <c r="AJ45" s="8"/>
+      <c r="AI45" s="8">
+        <v>1</v>
+      </c>
+      <c r="AJ45" s="8">
+        <v>2</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="46" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI46" s="8"/>
-      <c r="AJ46" s="8"/>
+      <c r="AI46" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ46" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI47" s="8"/>
+      <c r="AJ47" s="8"/>
+    </row>
+    <row r="48" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI48" s="8"/>
+      <c r="AJ48" s="8"/>
+    </row>
+    <row r="49" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI49" s="8"/>
+      <c r="AJ49" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -6955,7 +7010,7 @@
       <c r="I3" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="39">
+      <c r="J3" s="35">
         <f>(G6+G8+G10+G11+G12)</f>
         <v>111</v>
       </c>
@@ -6974,7 +7029,7 @@
       <c r="B4" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="35">
         <v>10000</v>
       </c>
       <c r="F4" t="str">
@@ -7007,7 +7062,7 @@
       <c r="B5" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="35">
         <v>1000000</v>
       </c>
       <c r="F5" t="str">
@@ -7040,7 +7095,7 @@
       <c r="B6" t="s">
         <v>183</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="35">
         <v>1100000</v>
       </c>
       <c r="F6" t="str">
@@ -7073,7 +7128,7 @@
       <c r="B7" t="s">
         <v>183</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="35">
         <v>10000</v>
       </c>
       <c r="F7" t="str">
@@ -7099,7 +7154,7 @@
       <c r="B8" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="35">
         <v>1000</v>
       </c>
       <c r="F8" t="str">
@@ -7118,7 +7173,7 @@
       <c r="B9" t="s">
         <v>183</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="35">
         <v>100</v>
       </c>
       <c r="F9" t="str">
@@ -7137,7 +7192,7 @@
       <c r="B10" t="s">
         <v>183</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="35">
         <v>100</v>
       </c>
       <c r="F10" t="str">
@@ -7156,7 +7211,7 @@
       <c r="B11" t="s">
         <v>183</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="35">
         <v>10</v>
       </c>
       <c r="F11" t="str">
@@ -7175,7 +7230,7 @@
       <c r="B12" t="s">
         <v>183</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="35">
         <v>1</v>
       </c>
       <c r="F12" t="str">
@@ -8877,7 +8932,7 @@
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8905,7 +8960,7 @@
         <f>D3+E$2</f>
         <v>99840</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="36">
         <f>E3+256</f>
         <v>100096</v>
       </c>
@@ -8925,7 +8980,7 @@
         <f t="shared" ref="E4:E12" si="1">D4+E$2</f>
         <v>100864</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="36">
         <f t="shared" ref="F4:F12" si="2">E4+256</f>
         <v>101120</v>
       </c>
@@ -8945,7 +9000,7 @@
         <f t="shared" si="1"/>
         <v>101888</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="36">
         <f t="shared" si="2"/>
         <v>102144</v>
       </c>
@@ -8965,7 +9020,7 @@
         <f t="shared" si="1"/>
         <v>100352</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="36">
         <f t="shared" si="2"/>
         <v>100608</v>
       </c>
@@ -8985,7 +9040,7 @@
         <f t="shared" si="1"/>
         <v>101376</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="36">
         <f t="shared" si="2"/>
         <v>101632</v>
       </c>
@@ -9005,7 +9060,7 @@
         <f t="shared" si="1"/>
         <v>100096</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="36">
         <f t="shared" si="2"/>
         <v>100352</v>
       </c>
@@ -9025,7 +9080,7 @@
         <f t="shared" si="1"/>
         <v>101120</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="36">
         <f t="shared" si="2"/>
         <v>101376</v>
       </c>
@@ -9045,7 +9100,7 @@
         <f t="shared" si="1"/>
         <v>102144</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="36">
         <f t="shared" si="2"/>
         <v>102400</v>
       </c>
@@ -9065,7 +9120,7 @@
         <f t="shared" si="1"/>
         <v>100608</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="36">
         <f t="shared" si="2"/>
         <v>100864</v>
       </c>
@@ -9085,9 +9140,388 @@
         <f t="shared" si="1"/>
         <v>101632</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="36">
         <f t="shared" si="2"/>
         <v>101888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE52E46-8F05-47F7-9C53-8EFF0B1B5D51}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="8"/>
+    <col min="3" max="3" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" ref="C4" si="0">HEX2DEC(B4)</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" ref="F4" si="1">HEX2DEC(E4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="45" t="str">
+        <f>DEC2HEX(C5)</f>
+        <v>2800</v>
+      </c>
+      <c r="C5" s="8">
+        <f>C12*C4</f>
+        <v>10240</v>
+      </c>
+      <c r="E5" s="45" t="str">
+        <f>DEC2HEX(F5)</f>
+        <v>2400</v>
+      </c>
+      <c r="F5" s="8">
+        <f>F12*F4</f>
+        <v>9216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2800</v>
+      </c>
+      <c r="C6" s="8">
+        <f>HEX2DEC(B6)</f>
+        <v>10240</v>
+      </c>
+      <c r="E6" s="8">
+        <v>4800</v>
+      </c>
+      <c r="F6" s="8">
+        <f>HEX2DEC(E6)</f>
+        <v>18432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="8">
+        <v>800</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" ref="C7:C15" si="2">HEX2DEC(B7)</f>
+        <v>2048</v>
+      </c>
+      <c r="E7" s="8">
+        <v>800</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" ref="F7:F15" si="3">HEX2DEC(E7)</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2000</v>
+      </c>
+      <c r="C9" s="8">
+        <f t="shared" si="2"/>
+        <v>8192</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="3"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="8">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>9</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" s="8">
+        <v>400</v>
+      </c>
+      <c r="C11" s="8">
+        <f t="shared" si="2"/>
+        <v>1024</v>
+      </c>
+      <c r="E11" s="8">
+        <v>200</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="3"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" s="45" t="str">
+        <f>DEC2HEX(C12)</f>
+        <v>1400</v>
+      </c>
+      <c r="C12" s="8">
+        <f>C10*C11</f>
+        <v>5120</v>
+      </c>
+      <c r="E12" s="45" t="str">
+        <f>DEC2HEX(F12)</f>
+        <v>1200</v>
+      </c>
+      <c r="F12" s="8">
+        <f>F10*F11</f>
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13" s="8">
+        <v>50</v>
+      </c>
+      <c r="C13" s="8">
+        <f>HEX2DEC(B13)</f>
+        <v>80</v>
+      </c>
+      <c r="E13" s="8">
+        <v>50</v>
+      </c>
+      <c r="F13" s="8">
+        <f>HEX2DEC(E13)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E14" s="8">
+        <v>2</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="8">
+        <v>4</v>
+      </c>
+      <c r="C15" s="8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E15" s="8">
+        <v>2</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>263</v>
+      </c>
+      <c r="B16" s="45" t="str">
+        <f>DEC2HEX(C16)</f>
+        <v>4800</v>
+      </c>
+      <c r="C16" s="8">
+        <f>C15*C$7+C$6</f>
+        <v>18432</v>
+      </c>
+      <c r="E16" s="45" t="str">
+        <f>DEC2HEX(F16)</f>
+        <v>5800</v>
+      </c>
+      <c r="F16" s="8">
+        <f>F15*F$7+F$6</f>
+        <v>22528</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" s="8">
+        <f>C9/C7-1</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8">
+        <f>F9/F7-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="46">
+        <f>C13*C14*C10*C11</f>
+        <v>819200</v>
+      </c>
+      <c r="F19" s="46">
+        <f>F13*F14*F10*F11</f>
+        <v>737280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>265</v>
+      </c>
+      <c r="B21" s="8">
+        <v>4</v>
+      </c>
+      <c r="C21" s="8">
+        <v>8</v>
+      </c>
+      <c r="E21" s="8">
+        <v>14</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" ref="F21" si="4">HEX2DEC(E21)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B22" s="45" t="str">
+        <f>DEC2HEX(C22)</f>
+        <v>6800</v>
+      </c>
+      <c r="C22" s="8">
+        <f>C21*C$7+C$6</f>
+        <v>26624</v>
+      </c>
+      <c r="E22" s="45" t="str">
+        <f>DEC2HEX(F22)</f>
+        <v>E800</v>
+      </c>
+      <c r="F22" s="8">
+        <f>F21*F$7+F$6</f>
+        <v>59392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed (final?) filecreate table reference
</commit_message>
<xml_diff>
--- a/DiskUtility/Notes/Skew Table.xlsx
+++ b/DiskUtility/Notes/Skew Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\Github\DiskImageUtility\DiskUtility\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFDF1A5-D5E9-4925-8DD9-CC3D4C472737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC79D89-B46F-4CCF-9FF6-7B62F3E13C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29955" yWindow="3420" windowWidth="21600" windowHeight="11385" activeTab="8" xr2:uid="{DD7A5C08-DCA6-4B6E-BD23-734986915BC7}"/>
+    <workbookView xWindow="2895" yWindow="0" windowWidth="24360" windowHeight="14505" activeTab="8" xr2:uid="{DD7A5C08-DCA6-4B6E-BD23-734986915BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Skew" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="276">
   <si>
     <t>Skew</t>
   </si>
@@ -843,6 +843,33 @@
   </si>
   <si>
     <t>File Offset</t>
+  </si>
+  <si>
+    <t>H17</t>
+  </si>
+  <si>
+    <t>1e00</t>
+  </si>
+  <si>
+    <t>BIOS.ASM</t>
+  </si>
+  <si>
+    <t>Start of Directory</t>
+  </si>
+  <si>
+    <t>Interleave</t>
+  </si>
+  <si>
+    <t>DIU</t>
+  </si>
+  <si>
+    <t>4, 0-3</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Track</t>
   </si>
 </sst>
 </file>
@@ -1093,11 +1120,13 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -6218,10 +6247,6 @@
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="N19" s="8"/>
-      <c r="T19" s="44"/>
-      <c r="U19" s="44"/>
-      <c r="V19" s="44"/>
-      <c r="W19" s="44"/>
       <c r="X19" s="41"/>
       <c r="Y19" s="8"/>
       <c r="AA19" s="42"/>
@@ -6236,10 +6261,6 @@
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
-      <c r="T20" s="44"/>
-      <c r="U20" s="44"/>
-      <c r="V20" s="44"/>
-      <c r="W20" s="44"/>
       <c r="X20" s="41"/>
       <c r="Y20" s="8"/>
       <c r="AA20" s="42"/>
@@ -6254,10 +6275,6 @@
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="T21" s="44"/>
-      <c r="U21" s="44"/>
-      <c r="V21" s="44"/>
-      <c r="W21" s="44"/>
       <c r="X21" s="41"/>
       <c r="Y21" s="8"/>
       <c r="AA21" s="42"/>
@@ -9152,10 +9169,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE52E46-8F05-47F7-9C53-8EFF0B1B5D51}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31:Y31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9164,9 +9181,13 @@
     <col min="2" max="2" width="9.140625" style="8"/>
     <col min="3" max="3" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="8"/>
+    <col min="14" max="14" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>252</v>
       </c>
@@ -9174,12 +9195,21 @@
         <v>251</v>
       </c>
       <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>271</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>72</v>
       </c>
@@ -9192,8 +9222,32 @@
       <c r="F3" s="8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>257</v>
       </c>
@@ -9211,12 +9265,46 @@
         <f t="shared" ref="F4" si="1">HEX2DEC(E4)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="8">
+        <v>2</v>
+      </c>
+      <c r="I4" s="8">
+        <f t="shared" ref="I4" si="2">HEX2DEC(H4)</f>
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>275</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="8">
+        <f>L8</f>
+        <v>7680</v>
+      </c>
+      <c r="S4" s="8" t="str">
+        <f t="shared" ref="S4:S13" si="3">DEC2HEX(R4)</f>
+        <v>1E00</v>
+      </c>
+      <c r="V4" s="8">
+        <v>7680</v>
+      </c>
+      <c r="W4" s="8" t="str">
+        <f t="shared" ref="W4:W23" si="4">DEC2HEX(V4)</f>
+        <v>1E00</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>258</v>
       </c>
-      <c r="B5" s="45" t="str">
+      <c r="B5" s="44" t="str">
         <f>DEC2HEX(C5)</f>
         <v>2800</v>
       </c>
@@ -9224,7 +9312,7 @@
         <f>C12*C4</f>
         <v>10240</v>
       </c>
-      <c r="E5" s="45" t="str">
+      <c r="E5" s="44" t="str">
         <f>DEC2HEX(F5)</f>
         <v>2400</v>
       </c>
@@ -9232,8 +9320,44 @@
         <f>F12*F4</f>
         <v>9216</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="44" t="str">
+        <f>DEC2HEX(I5)</f>
+        <v>1E00</v>
+      </c>
+      <c r="I5" s="8">
+        <v>7680</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0</v>
+      </c>
+      <c r="M5" s="8" t="str">
+        <f>DEC2HEX(L5)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <f>R$4+Q5*256</f>
+        <v>8192</v>
+      </c>
+      <c r="S5" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>2000</v>
+      </c>
+      <c r="V5">
+        <f>V4+256</f>
+        <v>7936</v>
+      </c>
+      <c r="W5" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>1F00</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>253</v>
       </c>
@@ -9251,8 +9375,44 @@
         <f>HEX2DEC(E6)</f>
         <v>18432</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="I6" s="8">
+        <f>HEX2DEC(H6)</f>
+        <v>7680</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8">
+        <v>2560</v>
+      </c>
+      <c r="M6" s="8" t="str">
+        <f>DEC2HEX(L6)</f>
+        <v>A00</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R13" si="5">R$4+Q6*256</f>
+        <v>8704</v>
+      </c>
+      <c r="S6" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>2200</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ref="V6:V23" si="6">V5+256</f>
+        <v>8192</v>
+      </c>
+      <c r="W6" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -9260,18 +9420,55 @@
         <v>800</v>
       </c>
       <c r="C7" s="8">
-        <f t="shared" ref="C7:C15" si="2">HEX2DEC(B7)</f>
+        <f t="shared" ref="C7:C15" si="7">HEX2DEC(B7)</f>
         <v>2048</v>
       </c>
       <c r="E7" s="8">
         <v>800</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" ref="F7:F15" si="3">HEX2DEC(E7)</f>
+        <f t="shared" ref="F7:F15" si="8">HEX2DEC(E7)</f>
         <v>2048</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" s="8">
+        <v>400</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" ref="I7:I15" si="9">HEX2DEC(H7)</f>
+        <v>1024</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="8">
+        <f>L6+L$6</f>
+        <v>5120</v>
+      </c>
+      <c r="M7" s="8" t="str">
+        <f t="shared" ref="M7:M14" si="10">DEC2HEX(L7)</f>
+        <v>1400</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="5"/>
+        <v>9216</v>
+      </c>
+      <c r="S7" s="46" t="str">
+        <f t="shared" si="3"/>
+        <v>2400</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="6"/>
+        <v>8448</v>
+      </c>
+      <c r="W7" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>264</v>
       </c>
@@ -9279,18 +9476,61 @@
         <v>2</v>
       </c>
       <c r="C8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E8" s="8">
         <v>2</v>
       </c>
       <c r="F8" s="8">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8" s="8">
+        <f>L7+L$6</f>
+        <v>7680</v>
+      </c>
+      <c r="M8" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>1E00</v>
+      </c>
+      <c r="N8" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="5"/>
+        <v>9728</v>
+      </c>
+      <c r="S8" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2600</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="6"/>
+        <v>8704</v>
+      </c>
+      <c r="W8" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2200</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>166</v>
       </c>
@@ -9298,18 +9538,55 @@
         <v>2000</v>
       </c>
       <c r="C9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>8192</v>
       </c>
       <c r="E9" s="8">
         <v>1000</v>
       </c>
       <c r="F9" s="8">
+        <f t="shared" si="8"/>
+        <v>4096</v>
+      </c>
+      <c r="H9" s="8">
+        <v>800</v>
+      </c>
+      <c r="I9" s="8">
+        <f t="shared" si="9"/>
+        <v>2048</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" s="8">
+        <f>L8+L$6</f>
+        <v>10240</v>
+      </c>
+      <c r="M9" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>2800</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="5"/>
+        <v>7936</v>
+      </c>
+      <c r="S9" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1F00</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="6"/>
+        <v>8960</v>
+      </c>
+      <c r="W9" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>137</v>
       </c>
@@ -9317,18 +9594,55 @@
         <v>5</v>
       </c>
       <c r="C10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="E10" s="8">
         <v>9</v>
       </c>
       <c r="F10" s="8">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="I10" s="8">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10" s="8">
+        <f>L9+L$6</f>
+        <v>12800</v>
+      </c>
+      <c r="M10" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>3200</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="5"/>
+        <v>8448</v>
+      </c>
+      <c r="S10" s="46" t="str">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2100</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="6"/>
+        <v>9216</v>
+      </c>
+      <c r="W10" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>254</v>
       </c>
@@ -9336,22 +9650,62 @@
         <v>400</v>
       </c>
       <c r="C11" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1024</v>
       </c>
       <c r="E11" s="8">
         <v>200</v>
       </c>
       <c r="F11" s="8">
+        <f t="shared" si="8"/>
+        <v>512</v>
+      </c>
+      <c r="H11" s="8">
+        <v>100</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" si="9"/>
+        <v>256</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11" s="8">
+        <f>L10+L$6</f>
+        <v>15360</v>
+      </c>
+      <c r="M11" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>3C00</v>
+      </c>
+      <c r="Q11">
+        <v>5</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="5"/>
+        <v>8960</v>
+      </c>
+      <c r="S11" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2300</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="6"/>
+        <v>9472</v>
+      </c>
+      <c r="W11" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2500</v>
+      </c>
+      <c r="X11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>260</v>
       </c>
-      <c r="B12" s="45" t="str">
+      <c r="B12" s="44" t="str">
         <f>DEC2HEX(C12)</f>
         <v>1400</v>
       </c>
@@ -9359,7 +9713,7 @@
         <f>C10*C11</f>
         <v>5120</v>
       </c>
-      <c r="E12" s="45" t="str">
+      <c r="E12" s="44" t="str">
         <f>DEC2HEX(F12)</f>
         <v>1200</v>
       </c>
@@ -9367,8 +9721,48 @@
         <f>F10*F11</f>
         <v>4608</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="44" t="str">
+        <f>DEC2HEX(I12)</f>
+        <v>A00</v>
+      </c>
+      <c r="I12" s="8">
+        <v>2560</v>
+      </c>
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12" s="8">
+        <f>L11+L$6</f>
+        <v>17920</v>
+      </c>
+      <c r="M12" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>4600</v>
+      </c>
+      <c r="Q12">
+        <v>7</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="5"/>
+        <v>9472</v>
+      </c>
+      <c r="S12" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>2500</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="6"/>
+        <v>9728</v>
+      </c>
+      <c r="W12" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>259</v>
       </c>
@@ -9386,8 +9780,47 @@
         <f>HEX2DEC(E13)</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" s="8">
+        <v>50</v>
+      </c>
+      <c r="I13" s="8">
+        <v>40</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="L13" s="8">
+        <f>L12+L$6</f>
+        <v>20480</v>
+      </c>
+      <c r="M13" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>5000</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>9</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="5"/>
+        <v>9984</v>
+      </c>
+      <c r="S13" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>2700</v>
+      </c>
+      <c r="T13">
+        <v>2</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="6"/>
+        <v>9984</v>
+      </c>
+      <c r="W13" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>255</v>
       </c>
@@ -9395,18 +9828,54 @@
         <v>2</v>
       </c>
       <c r="C14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E14" s="8">
         <v>2</v>
       </c>
       <c r="F14" s="8">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="H14" s="8">
+        <v>2</v>
+      </c>
+      <c r="I14" s="8">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>9</v>
+      </c>
+      <c r="L14" s="8">
+        <f>L13+L$6</f>
+        <v>23040</v>
+      </c>
+      <c r="M14" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>5A00</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14" s="8">
+        <f>L9</f>
+        <v>10240</v>
+      </c>
+      <c r="S14" s="8" t="str">
+        <f t="shared" ref="S14:S23" si="11">DEC2HEX(R14)</f>
+        <v>2800</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="6"/>
+        <v>10240</v>
+      </c>
+      <c r="W14" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>256</v>
       </c>
@@ -9414,22 +9883,47 @@
         <v>4</v>
       </c>
       <c r="C15" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="E15" s="8">
         <v>2</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="H15" s="8">
+        <v>4</v>
+      </c>
+      <c r="I15" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15">
+        <f>R$14+Q15*256</f>
+        <v>11008</v>
+      </c>
+      <c r="S15" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>2B00</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="6"/>
+        <v>10496</v>
+      </c>
+      <c r="W15" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>263</v>
       </c>
-      <c r="B16" s="45" t="str">
+      <c r="B16" s="44" t="str">
         <f>DEC2HEX(C16)</f>
         <v>4800</v>
       </c>
@@ -9437,7 +9931,7 @@
         <f>C15*C$7+C$6</f>
         <v>18432</v>
       </c>
-      <c r="E16" s="45" t="str">
+      <c r="E16" s="44" t="str">
         <f>DEC2HEX(F16)</f>
         <v>5800</v>
       </c>
@@ -9445,8 +9939,35 @@
         <f>F15*F$7+F$6</f>
         <v>22528</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" s="44" t="str">
+        <f>DEC2HEX(I16)</f>
+        <v>2600</v>
+      </c>
+      <c r="I16" s="8">
+        <f>I15*I$7+I$6</f>
+        <v>9728</v>
+      </c>
+      <c r="Q16">
+        <v>6</v>
+      </c>
+      <c r="R16">
+        <f>R$14+Q16*256</f>
+        <v>11776</v>
+      </c>
+      <c r="S16" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>2E00</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="6"/>
+        <v>10752</v>
+      </c>
+      <c r="W16" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2A00</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>261</v>
       </c>
@@ -9457,8 +9978,30 @@
       <c r="F17" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>9</v>
+      </c>
+      <c r="R17">
+        <f>R$14+Q17*256</f>
+        <v>12544</v>
+      </c>
+      <c r="S17" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>3100</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="6"/>
+        <v>11008</v>
+      </c>
+      <c r="W17" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2B00</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>262</v>
       </c>
@@ -9471,21 +10014,88 @@
         <f>F9/F7-1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I18" s="8">
+        <f>I9/I7-1</f>
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <f>R$14+Q18*256</f>
+        <v>10752</v>
+      </c>
+      <c r="S18" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>2A00</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="6"/>
+        <v>11264</v>
+      </c>
+      <c r="W18" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2C00</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="45">
         <f>C13*C14*C10*C11</f>
         <v>819200</v>
       </c>
-      <c r="F19" s="46">
+      <c r="F19" s="45">
         <f>F13*F14*F10*F11</f>
         <v>737280</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I19" s="45">
+        <f>I13*I14*I10*I11</f>
+        <v>102400</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19">
+        <f>R$14+Q19*256</f>
+        <v>11520</v>
+      </c>
+      <c r="S19" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>2D00</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="6"/>
+        <v>11520</v>
+      </c>
+      <c r="W19" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2D00</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>8</v>
+      </c>
+      <c r="R20">
+        <f>R$14+Q20*256</f>
+        <v>12288</v>
+      </c>
+      <c r="S20" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>3000</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="6"/>
+        <v>11776</v>
+      </c>
+      <c r="W20" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2E00</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>265</v>
       </c>
@@ -9499,15 +10109,40 @@
         <v>14</v>
       </c>
       <c r="F21" s="8">
-        <f t="shared" ref="F21" si="4">HEX2DEC(E21)</f>
+        <f t="shared" ref="F21" si="12">HEX2DEC(E21)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" s="8">
+        <v>4</v>
+      </c>
+      <c r="I21" s="8">
+        <v>8</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <f>R$14+Q21*256</f>
+        <v>10496</v>
+      </c>
+      <c r="S21" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>2900</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="6"/>
+        <v>12032</v>
+      </c>
+      <c r="W21" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>2F00</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>266</v>
       </c>
-      <c r="B22" s="45" t="str">
+      <c r="B22" s="44" t="str">
         <f>DEC2HEX(C22)</f>
         <v>6800</v>
       </c>
@@ -9515,13 +10150,202 @@
         <f>C21*C$7+C$6</f>
         <v>26624</v>
       </c>
-      <c r="E22" s="45" t="str">
+      <c r="E22" s="44" t="str">
         <f>DEC2HEX(F22)</f>
         <v>E800</v>
       </c>
       <c r="F22" s="8">
         <f>F21*F$7+F$6</f>
         <v>59392</v>
+      </c>
+      <c r="H22" s="44" t="str">
+        <f>DEC2HEX(I22)</f>
+        <v>3E00</v>
+      </c>
+      <c r="I22" s="8">
+        <f>I21*I$7+I$6</f>
+        <v>15872</v>
+      </c>
+      <c r="Q22">
+        <v>4</v>
+      </c>
+      <c r="R22">
+        <f>R$14+Q22*256</f>
+        <v>11264</v>
+      </c>
+      <c r="S22" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>2C00</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="6"/>
+        <v>12288</v>
+      </c>
+      <c r="W22" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>7</v>
+      </c>
+      <c r="R23">
+        <f>R$14+Q23*256</f>
+        <v>12032</v>
+      </c>
+      <c r="S23" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>2F00</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="6"/>
+        <v>12544</v>
+      </c>
+      <c r="W23" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>3</v>
+      </c>
+      <c r="R26">
+        <v>6</v>
+      </c>
+      <c r="S26">
+        <v>9</v>
+      </c>
+      <c r="T26">
+        <v>2</v>
+      </c>
+      <c r="U26">
+        <v>5</v>
+      </c>
+      <c r="V26">
+        <v>8</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>4</v>
+      </c>
+      <c r="Y26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
+      <c r="R27">
+        <v>4</v>
+      </c>
+      <c r="S27">
+        <v>6</v>
+      </c>
+      <c r="T27" s="2">
+        <v>8</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>3</v>
+      </c>
+      <c r="W27">
+        <v>5</v>
+      </c>
+      <c r="X27">
+        <v>7</v>
+      </c>
+      <c r="Y27" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>5</v>
+      </c>
+      <c r="R29">
+        <v>9</v>
+      </c>
+      <c r="S29">
+        <v>3</v>
+      </c>
+      <c r="T29">
+        <v>7</v>
+      </c>
+      <c r="U29">
+        <v>2</v>
+      </c>
+      <c r="V29">
+        <v>6</v>
+      </c>
+      <c r="W29">
+        <v>10</v>
+      </c>
+      <c r="X29">
+        <v>4</v>
+      </c>
+      <c r="Y29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>4</v>
+      </c>
+      <c r="R31">
+        <v>8</v>
+      </c>
+      <c r="S31">
+        <v>2</v>
+      </c>
+      <c r="T31">
+        <v>6</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>5</v>
+      </c>
+      <c r="W31">
+        <v>9</v>
+      </c>
+      <c r="X31">
+        <v>3</v>
+      </c>
+      <c r="Y31">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>